<commit_message>
agregar y modificar imagen mas metadata listo
</commit_message>
<xml_diff>
--- a/DB_PAPILA/ClinicalData/patient_data_od.xlsx
+++ b/DB_PAPILA/ClinicalData/patient_data_od.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M246"/>
+  <dimension ref="A1:M251"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -501,13 +501,15 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="1" t="inlineStr">
         <is>
           <t>#002</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>47</v>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -542,7 +544,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="1" t="inlineStr">
         <is>
           <t>#004</t>
         </is>
@@ -583,7 +585,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="1" t="inlineStr">
         <is>
           <t>#005</t>
         </is>
@@ -626,7 +628,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="1" t="inlineStr">
         <is>
           <t>#006</t>
         </is>
@@ -667,7 +669,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="1" t="inlineStr">
         <is>
           <t>#007</t>
         </is>
@@ -706,7 +708,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="1" t="inlineStr">
         <is>
           <t>#008</t>
         </is>
@@ -745,7 +747,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" s="1" t="inlineStr">
         <is>
           <t>#009</t>
         </is>
@@ -786,7 +788,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" s="1" t="inlineStr">
         <is>
           <t>#010</t>
         </is>
@@ -827,7 +829,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" s="1" t="inlineStr">
         <is>
           <t>#013</t>
         </is>
@@ -870,7 +872,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" s="1" t="inlineStr">
         <is>
           <t>#014</t>
         </is>
@@ -913,7 +915,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="A12" s="1" t="inlineStr">
         <is>
           <t>#015</t>
         </is>
@@ -956,7 +958,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="A13" s="1" t="inlineStr">
         <is>
           <t>#016</t>
         </is>
@@ -997,7 +999,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="A14" s="1" t="inlineStr">
         <is>
           <t>#018</t>
         </is>
@@ -1038,7 +1040,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
+      <c r="A15" s="1" t="inlineStr">
         <is>
           <t>#019</t>
         </is>
@@ -1075,7 +1077,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
+      <c r="A16" s="1" t="inlineStr">
         <is>
           <t>#020</t>
         </is>
@@ -1114,7 +1116,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
+      <c r="A17" s="1" t="inlineStr">
         <is>
           <t>#021</t>
         </is>
@@ -1153,7 +1155,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
+      <c r="A18" s="1" t="inlineStr">
         <is>
           <t>#023</t>
         </is>
@@ -1194,7 +1196,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
+      <c r="A19" s="1" t="inlineStr">
         <is>
           <t>#024</t>
         </is>
@@ -1237,7 +1239,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
+      <c r="A20" s="1" t="inlineStr">
         <is>
           <t>#025</t>
         </is>
@@ -1280,7 +1282,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
+      <c r="A21" s="1" t="inlineStr">
         <is>
           <t>#026</t>
         </is>
@@ -1321,7 +1323,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
+      <c r="A22" s="1" t="inlineStr">
         <is>
           <t>#027</t>
         </is>
@@ -1362,7 +1364,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
+      <c r="A23" s="1" t="inlineStr">
         <is>
           <t>#028</t>
         </is>
@@ -1401,7 +1403,7 @@
       <c r="M23" t="inlineStr"/>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
+      <c r="A24" s="1" t="inlineStr">
         <is>
           <t>#029</t>
         </is>
@@ -1440,7 +1442,7 @@
       <c r="M24" t="inlineStr"/>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
+      <c r="A25" s="1" t="inlineStr">
         <is>
           <t>#030</t>
         </is>
@@ -1479,7 +1481,7 @@
       <c r="M25" t="inlineStr"/>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
+      <c r="A26" s="1" t="inlineStr">
         <is>
           <t>#031</t>
         </is>
@@ -1518,7 +1520,7 @@
       <c r="M26" t="inlineStr"/>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
+      <c r="A27" s="1" t="inlineStr">
         <is>
           <t>#032</t>
         </is>
@@ -1557,7 +1559,7 @@
       <c r="M27" t="inlineStr"/>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
+      <c r="A28" s="1" t="inlineStr">
         <is>
           <t>#033</t>
         </is>
@@ -1596,7 +1598,7 @@
       <c r="M28" t="inlineStr"/>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
+      <c r="A29" s="1" t="inlineStr">
         <is>
           <t>#034</t>
         </is>
@@ -1635,7 +1637,7 @@
       <c r="M29" t="inlineStr"/>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
+      <c r="A30" s="1" t="inlineStr">
         <is>
           <t>#035</t>
         </is>
@@ -1674,7 +1676,7 @@
       <c r="M30" t="inlineStr"/>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
+      <c r="A31" s="1" t="inlineStr">
         <is>
           <t>#036</t>
         </is>
@@ -1713,7 +1715,7 @@
       <c r="M31" t="inlineStr"/>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
+      <c r="A32" s="1" t="inlineStr">
         <is>
           <t>#037</t>
         </is>
@@ -1748,7 +1750,7 @@
       <c r="M32" t="inlineStr"/>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
+      <c r="A33" s="1" t="inlineStr">
         <is>
           <t>#038</t>
         </is>
@@ -1785,7 +1787,7 @@
       <c r="M33" t="inlineStr"/>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr">
+      <c r="A34" s="1" t="inlineStr">
         <is>
           <t>#039</t>
         </is>
@@ -1824,7 +1826,7 @@
       <c r="M34" t="inlineStr"/>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr">
+      <c r="A35" s="1" t="inlineStr">
         <is>
           <t>#041</t>
         </is>
@@ -1865,7 +1867,7 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr">
+      <c r="A36" s="1" t="inlineStr">
         <is>
           <t>#042</t>
         </is>
@@ -1906,7 +1908,7 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr">
+      <c r="A37" s="1" t="inlineStr">
         <is>
           <t>#044</t>
         </is>
@@ -1947,7 +1949,7 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
+      <c r="A38" s="1" t="inlineStr">
         <is>
           <t>#045</t>
         </is>
@@ -1990,7 +1992,7 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr">
+      <c r="A39" s="1" t="inlineStr">
         <is>
           <t>#046</t>
         </is>
@@ -2029,7 +2031,7 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr">
+      <c r="A40" s="1" t="inlineStr">
         <is>
           <t>#047</t>
         </is>
@@ -2070,7 +2072,7 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr">
+      <c r="A41" s="1" t="inlineStr">
         <is>
           <t>#048</t>
         </is>
@@ -2111,7 +2113,7 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr">
+      <c r="A42" s="1" t="inlineStr">
         <is>
           <t>#050</t>
         </is>
@@ -2154,7 +2156,7 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="inlineStr">
+      <c r="A43" s="1" t="inlineStr">
         <is>
           <t>#051</t>
         </is>
@@ -2197,7 +2199,7 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="inlineStr">
+      <c r="A44" s="1" t="inlineStr">
         <is>
           <t>#053</t>
         </is>
@@ -2238,7 +2240,7 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr">
+      <c r="A45" s="1" t="inlineStr">
         <is>
           <t>#055</t>
         </is>
@@ -2279,7 +2281,7 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="inlineStr">
+      <c r="A46" s="1" t="inlineStr">
         <is>
           <t>#056</t>
         </is>
@@ -2320,7 +2322,7 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="inlineStr">
+      <c r="A47" s="1" t="inlineStr">
         <is>
           <t>#057</t>
         </is>
@@ -2359,7 +2361,7 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="inlineStr">
+      <c r="A48" s="1" t="inlineStr">
         <is>
           <t>#062</t>
         </is>
@@ -2400,7 +2402,7 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="inlineStr">
+      <c r="A49" s="1" t="inlineStr">
         <is>
           <t>#064</t>
         </is>
@@ -2439,7 +2441,7 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="inlineStr">
+      <c r="A50" s="1" t="inlineStr">
         <is>
           <t>#065</t>
         </is>
@@ -2480,7 +2482,7 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="inlineStr">
+      <c r="A51" s="1" t="inlineStr">
         <is>
           <t>#066</t>
         </is>
@@ -2523,7 +2525,7 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="inlineStr">
+      <c r="A52" s="1" t="inlineStr">
         <is>
           <t>#067</t>
         </is>
@@ -2564,7 +2566,7 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="inlineStr">
+      <c r="A53" s="1" t="inlineStr">
         <is>
           <t>#068</t>
         </is>
@@ -2605,7 +2607,7 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="inlineStr">
+      <c r="A54" s="1" t="inlineStr">
         <is>
           <t>#069</t>
         </is>
@@ -2646,7 +2648,7 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" t="inlineStr">
+      <c r="A55" s="1" t="inlineStr">
         <is>
           <t>#072</t>
         </is>
@@ -2683,7 +2685,7 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" t="inlineStr">
+      <c r="A56" s="1" t="inlineStr">
         <is>
           <t>#073</t>
         </is>
@@ -2724,7 +2726,7 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" t="inlineStr">
+      <c r="A57" s="1" t="inlineStr">
         <is>
           <t>#074</t>
         </is>
@@ -2765,7 +2767,7 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" t="inlineStr">
+      <c r="A58" s="1" t="inlineStr">
         <is>
           <t>#077</t>
         </is>
@@ -2804,7 +2806,7 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="inlineStr">
+      <c r="A59" s="1" t="inlineStr">
         <is>
           <t>#079</t>
         </is>
@@ -2843,7 +2845,7 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="inlineStr">
+      <c r="A60" s="1" t="inlineStr">
         <is>
           <t>#081</t>
         </is>
@@ -2882,7 +2884,7 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" t="inlineStr">
+      <c r="A61" s="1" t="inlineStr">
         <is>
           <t>#084</t>
         </is>
@@ -2923,7 +2925,7 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" t="inlineStr">
+      <c r="A62" s="1" t="inlineStr">
         <is>
           <t>#087</t>
         </is>
@@ -2964,7 +2966,7 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" t="inlineStr">
+      <c r="A63" s="1" t="inlineStr">
         <is>
           <t>#088</t>
         </is>
@@ -3005,7 +3007,7 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" t="inlineStr">
+      <c r="A64" s="1" t="inlineStr">
         <is>
           <t>#089</t>
         </is>
@@ -3046,7 +3048,7 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" t="inlineStr">
+      <c r="A65" s="1" t="inlineStr">
         <is>
           <t>#090</t>
         </is>
@@ -3087,7 +3089,7 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" t="inlineStr">
+      <c r="A66" s="1" t="inlineStr">
         <is>
           <t>#091</t>
         </is>
@@ -3128,7 +3130,7 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" t="inlineStr">
+      <c r="A67" s="1" t="inlineStr">
         <is>
           <t>#092</t>
         </is>
@@ -3169,7 +3171,7 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" t="inlineStr">
+      <c r="A68" s="1" t="inlineStr">
         <is>
           <t>#093</t>
         </is>
@@ -3210,7 +3212,7 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" t="inlineStr">
+      <c r="A69" s="1" t="inlineStr">
         <is>
           <t>#096</t>
         </is>
@@ -3253,7 +3255,7 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" t="inlineStr">
+      <c r="A70" s="1" t="inlineStr">
         <is>
           <t>#098</t>
         </is>
@@ -3292,7 +3294,7 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" t="inlineStr">
+      <c r="A71" s="1" t="inlineStr">
         <is>
           <t>#101</t>
         </is>
@@ -3333,7 +3335,7 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" t="inlineStr">
+      <c r="A72" s="1" t="inlineStr">
         <is>
           <t>#102</t>
         </is>
@@ -3374,7 +3376,7 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" t="inlineStr">
+      <c r="A73" s="1" t="inlineStr">
         <is>
           <t>#104</t>
         </is>
@@ -3417,7 +3419,7 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" t="inlineStr">
+      <c r="A74" s="1" t="inlineStr">
         <is>
           <t>#105</t>
         </is>
@@ -3458,7 +3460,7 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" t="inlineStr">
+      <c r="A75" s="1" t="inlineStr">
         <is>
           <t>#106</t>
         </is>
@@ -3499,7 +3501,7 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" t="inlineStr">
+      <c r="A76" s="1" t="inlineStr">
         <is>
           <t>#107</t>
         </is>
@@ -3538,7 +3540,7 @@
       </c>
     </row>
     <row r="77">
-      <c r="A77" t="inlineStr">
+      <c r="A77" s="1" t="inlineStr">
         <is>
           <t>#108</t>
         </is>
@@ -3579,7 +3581,7 @@
       </c>
     </row>
     <row r="78">
-      <c r="A78" t="inlineStr">
+      <c r="A78" s="1" t="inlineStr">
         <is>
           <t>#112</t>
         </is>
@@ -3622,7 +3624,7 @@
       </c>
     </row>
     <row r="79">
-      <c r="A79" t="inlineStr">
+      <c r="A79" s="1" t="inlineStr">
         <is>
           <t>#113</t>
         </is>
@@ -3663,7 +3665,7 @@
       </c>
     </row>
     <row r="80">
-      <c r="A80" t="inlineStr">
+      <c r="A80" s="1" t="inlineStr">
         <is>
           <t>#114</t>
         </is>
@@ -3702,7 +3704,7 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" t="inlineStr">
+      <c r="A81" s="1" t="inlineStr">
         <is>
           <t>#116</t>
         </is>
@@ -3741,7 +3743,7 @@
       </c>
     </row>
     <row r="82">
-      <c r="A82" t="inlineStr">
+      <c r="A82" s="1" t="inlineStr">
         <is>
           <t>#119</t>
         </is>
@@ -3782,7 +3784,7 @@
       </c>
     </row>
     <row r="83">
-      <c r="A83" t="inlineStr">
+      <c r="A83" s="1" t="inlineStr">
         <is>
           <t>#120</t>
         </is>
@@ -3821,7 +3823,7 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" t="inlineStr">
+      <c r="A84" s="1" t="inlineStr">
         <is>
           <t>#121</t>
         </is>
@@ -3862,7 +3864,7 @@
       </c>
     </row>
     <row r="85">
-      <c r="A85" t="inlineStr">
+      <c r="A85" s="1" t="inlineStr">
         <is>
           <t>#122</t>
         </is>
@@ -3903,7 +3905,7 @@
       </c>
     </row>
     <row r="86">
-      <c r="A86" t="inlineStr">
+      <c r="A86" s="1" t="inlineStr">
         <is>
           <t>#123</t>
         </is>
@@ -3944,7 +3946,7 @@
       </c>
     </row>
     <row r="87">
-      <c r="A87" t="inlineStr">
+      <c r="A87" s="1" t="inlineStr">
         <is>
           <t>#124</t>
         </is>
@@ -3985,7 +3987,7 @@
       </c>
     </row>
     <row r="88">
-      <c r="A88" t="inlineStr">
+      <c r="A88" s="1" t="inlineStr">
         <is>
           <t>#125</t>
         </is>
@@ -4024,7 +4026,7 @@
       <c r="M88" t="inlineStr"/>
     </row>
     <row r="89">
-      <c r="A89" t="inlineStr">
+      <c r="A89" s="1" t="inlineStr">
         <is>
           <t>#126</t>
         </is>
@@ -4063,7 +4065,7 @@
       <c r="M89" t="inlineStr"/>
     </row>
     <row r="90">
-      <c r="A90" t="inlineStr">
+      <c r="A90" s="1" t="inlineStr">
         <is>
           <t>#127</t>
         </is>
@@ -4102,7 +4104,7 @@
       <c r="M90" t="inlineStr"/>
     </row>
     <row r="91">
-      <c r="A91" t="inlineStr">
+      <c r="A91" s="1" t="inlineStr">
         <is>
           <t>#128</t>
         </is>
@@ -4141,7 +4143,7 @@
       <c r="M91" t="inlineStr"/>
     </row>
     <row r="92">
-      <c r="A92" t="inlineStr">
+      <c r="A92" s="1" t="inlineStr">
         <is>
           <t>#129</t>
         </is>
@@ -4180,7 +4182,7 @@
       <c r="M92" t="inlineStr"/>
     </row>
     <row r="93">
-      <c r="A93" t="inlineStr">
+      <c r="A93" s="1" t="inlineStr">
         <is>
           <t>#130</t>
         </is>
@@ -4217,7 +4219,7 @@
       <c r="M93" t="inlineStr"/>
     </row>
     <row r="94">
-      <c r="A94" t="inlineStr">
+      <c r="A94" s="1" t="inlineStr">
         <is>
           <t>#131</t>
         </is>
@@ -4256,7 +4258,7 @@
       <c r="M94" t="inlineStr"/>
     </row>
     <row r="95">
-      <c r="A95" t="inlineStr">
+      <c r="A95" s="1" t="inlineStr">
         <is>
           <t>#132</t>
         </is>
@@ -4295,7 +4297,7 @@
       <c r="M95" t="inlineStr"/>
     </row>
     <row r="96">
-      <c r="A96" t="inlineStr">
+      <c r="A96" s="1" t="inlineStr">
         <is>
           <t>#133</t>
         </is>
@@ -4334,7 +4336,7 @@
       <c r="M96" t="inlineStr"/>
     </row>
     <row r="97">
-      <c r="A97" t="inlineStr">
+      <c r="A97" s="1" t="inlineStr">
         <is>
           <t>#134</t>
         </is>
@@ -4373,7 +4375,7 @@
       <c r="M97" t="inlineStr"/>
     </row>
     <row r="98">
-      <c r="A98" t="inlineStr">
+      <c r="A98" s="1" t="inlineStr">
         <is>
           <t>#135</t>
         </is>
@@ -4412,7 +4414,7 @@
       <c r="M98" t="inlineStr"/>
     </row>
     <row r="99">
-      <c r="A99" t="inlineStr">
+      <c r="A99" s="1" t="inlineStr">
         <is>
           <t>#136</t>
         </is>
@@ -4451,7 +4453,7 @@
       <c r="M99" t="inlineStr"/>
     </row>
     <row r="100">
-      <c r="A100" t="inlineStr">
+      <c r="A100" s="1" t="inlineStr">
         <is>
           <t>#137</t>
         </is>
@@ -4490,7 +4492,7 @@
       <c r="M100" t="inlineStr"/>
     </row>
     <row r="101">
-      <c r="A101" t="inlineStr">
+      <c r="A101" s="1" t="inlineStr">
         <is>
           <t>#138</t>
         </is>
@@ -4529,7 +4531,7 @@
       <c r="M101" t="inlineStr"/>
     </row>
     <row r="102">
-      <c r="A102" t="inlineStr">
+      <c r="A102" s="1" t="inlineStr">
         <is>
           <t>#139</t>
         </is>
@@ -4568,7 +4570,7 @@
       <c r="M102" t="inlineStr"/>
     </row>
     <row r="103">
-      <c r="A103" t="inlineStr">
+      <c r="A103" s="1" t="inlineStr">
         <is>
           <t>#140</t>
         </is>
@@ -4605,7 +4607,7 @@
       <c r="M103" t="inlineStr"/>
     </row>
     <row r="104">
-      <c r="A104" t="inlineStr">
+      <c r="A104" s="1" t="inlineStr">
         <is>
           <t>#141</t>
         </is>
@@ -4644,7 +4646,7 @@
       <c r="M104" t="inlineStr"/>
     </row>
     <row r="105">
-      <c r="A105" t="inlineStr">
+      <c r="A105" s="1" t="inlineStr">
         <is>
           <t>#142</t>
         </is>
@@ -4683,7 +4685,7 @@
       <c r="M105" t="inlineStr"/>
     </row>
     <row r="106">
-      <c r="A106" t="inlineStr">
+      <c r="A106" s="1" t="inlineStr">
         <is>
           <t>#143</t>
         </is>
@@ -4722,7 +4724,7 @@
       <c r="M106" t="inlineStr"/>
     </row>
     <row r="107">
-      <c r="A107" t="inlineStr">
+      <c r="A107" s="1" t="inlineStr">
         <is>
           <t>#144</t>
         </is>
@@ -4761,7 +4763,7 @@
       <c r="M107" t="inlineStr"/>
     </row>
     <row r="108">
-      <c r="A108" t="inlineStr">
+      <c r="A108" s="1" t="inlineStr">
         <is>
           <t>#146</t>
         </is>
@@ -4800,7 +4802,7 @@
       <c r="M108" t="inlineStr"/>
     </row>
     <row r="109">
-      <c r="A109" t="inlineStr">
+      <c r="A109" s="1" t="inlineStr">
         <is>
           <t>#147</t>
         </is>
@@ -4837,7 +4839,7 @@
       <c r="M109" t="inlineStr"/>
     </row>
     <row r="110">
-      <c r="A110" t="inlineStr">
+      <c r="A110" s="1" t="inlineStr">
         <is>
           <t>#149</t>
         </is>
@@ -4876,7 +4878,7 @@
       <c r="M110" t="inlineStr"/>
     </row>
     <row r="111">
-      <c r="A111" t="inlineStr">
+      <c r="A111" s="1" t="inlineStr">
         <is>
           <t>#150</t>
         </is>
@@ -4915,7 +4917,7 @@
       <c r="M111" t="inlineStr"/>
     </row>
     <row r="112">
-      <c r="A112" t="inlineStr">
+      <c r="A112" s="1" t="inlineStr">
         <is>
           <t>#151</t>
         </is>
@@ -4954,7 +4956,7 @@
       <c r="M112" t="inlineStr"/>
     </row>
     <row r="113">
-      <c r="A113" t="inlineStr">
+      <c r="A113" s="1" t="inlineStr">
         <is>
           <t>#152</t>
         </is>
@@ -4993,7 +4995,7 @@
       <c r="M113" t="inlineStr"/>
     </row>
     <row r="114">
-      <c r="A114" t="inlineStr">
+      <c r="A114" s="1" t="inlineStr">
         <is>
           <t>#153</t>
         </is>
@@ -5032,7 +5034,7 @@
       <c r="M114" t="inlineStr"/>
     </row>
     <row r="115">
-      <c r="A115" t="inlineStr">
+      <c r="A115" s="1" t="inlineStr">
         <is>
           <t>#154</t>
         </is>
@@ -5071,7 +5073,7 @@
       <c r="M115" t="inlineStr"/>
     </row>
     <row r="116">
-      <c r="A116" t="inlineStr">
+      <c r="A116" s="1" t="inlineStr">
         <is>
           <t>#155</t>
         </is>
@@ -5110,7 +5112,7 @@
       <c r="M116" t="inlineStr"/>
     </row>
     <row r="117">
-      <c r="A117" t="inlineStr">
+      <c r="A117" s="1" t="inlineStr">
         <is>
           <t>#156</t>
         </is>
@@ -5149,7 +5151,7 @@
       <c r="M117" t="inlineStr"/>
     </row>
     <row r="118">
-      <c r="A118" t="inlineStr">
+      <c r="A118" s="1" t="inlineStr">
         <is>
           <t>#157</t>
         </is>
@@ -5186,7 +5188,7 @@
       <c r="M118" t="inlineStr"/>
     </row>
     <row r="119">
-      <c r="A119" t="inlineStr">
+      <c r="A119" s="1" t="inlineStr">
         <is>
           <t>#158</t>
         </is>
@@ -5225,7 +5227,7 @@
       <c r="M119" t="inlineStr"/>
     </row>
     <row r="120">
-      <c r="A120" t="inlineStr">
+      <c r="A120" s="1" t="inlineStr">
         <is>
           <t>#159</t>
         </is>
@@ -5264,7 +5266,7 @@
       <c r="M120" t="inlineStr"/>
     </row>
     <row r="121">
-      <c r="A121" t="inlineStr">
+      <c r="A121" s="1" t="inlineStr">
         <is>
           <t>#160</t>
         </is>
@@ -5303,7 +5305,7 @@
       <c r="M121" t="inlineStr"/>
     </row>
     <row r="122">
-      <c r="A122" t="inlineStr">
+      <c r="A122" s="1" t="inlineStr">
         <is>
           <t>#162</t>
         </is>
@@ -5342,7 +5344,7 @@
       <c r="M122" t="inlineStr"/>
     </row>
     <row r="123">
-      <c r="A123" t="inlineStr">
+      <c r="A123" s="1" t="inlineStr">
         <is>
           <t>#163</t>
         </is>
@@ -5381,7 +5383,7 @@
       <c r="M123" t="inlineStr"/>
     </row>
     <row r="124">
-      <c r="A124" t="inlineStr">
+      <c r="A124" s="1" t="inlineStr">
         <is>
           <t>#164</t>
         </is>
@@ -5420,7 +5422,7 @@
       <c r="M124" t="inlineStr"/>
     </row>
     <row r="125">
-      <c r="A125" t="inlineStr">
+      <c r="A125" s="1" t="inlineStr">
         <is>
           <t>#165</t>
         </is>
@@ -5459,7 +5461,7 @@
       <c r="M125" t="inlineStr"/>
     </row>
     <row r="126">
-      <c r="A126" t="inlineStr">
+      <c r="A126" s="1" t="inlineStr">
         <is>
           <t>#166</t>
         </is>
@@ -5498,7 +5500,7 @@
       <c r="M126" t="inlineStr"/>
     </row>
     <row r="127">
-      <c r="A127" t="inlineStr">
+      <c r="A127" s="1" t="inlineStr">
         <is>
           <t>#168</t>
         </is>
@@ -5537,7 +5539,7 @@
       <c r="M127" t="inlineStr"/>
     </row>
     <row r="128">
-      <c r="A128" t="inlineStr">
+      <c r="A128" s="1" t="inlineStr">
         <is>
           <t>#169</t>
         </is>
@@ -5576,7 +5578,7 @@
       <c r="M128" t="inlineStr"/>
     </row>
     <row r="129">
-      <c r="A129" t="inlineStr">
+      <c r="A129" s="1" t="inlineStr">
         <is>
           <t>#170</t>
         </is>
@@ -5615,7 +5617,7 @@
       <c r="M129" t="inlineStr"/>
     </row>
     <row r="130">
-      <c r="A130" t="inlineStr">
+      <c r="A130" s="1" t="inlineStr">
         <is>
           <t>#171</t>
         </is>
@@ -5654,7 +5656,7 @@
       <c r="M130" t="inlineStr"/>
     </row>
     <row r="131">
-      <c r="A131" t="inlineStr">
+      <c r="A131" s="1" t="inlineStr">
         <is>
           <t>#172</t>
         </is>
@@ -5693,7 +5695,7 @@
       <c r="M131" t="inlineStr"/>
     </row>
     <row r="132">
-      <c r="A132" t="inlineStr">
+      <c r="A132" s="1" t="inlineStr">
         <is>
           <t>#174</t>
         </is>
@@ -5732,7 +5734,7 @@
       <c r="M132" t="inlineStr"/>
     </row>
     <row r="133">
-      <c r="A133" t="inlineStr">
+      <c r="A133" s="1" t="inlineStr">
         <is>
           <t>#175</t>
         </is>
@@ -5771,7 +5773,7 @@
       <c r="M133" t="inlineStr"/>
     </row>
     <row r="134">
-      <c r="A134" t="inlineStr">
+      <c r="A134" s="1" t="inlineStr">
         <is>
           <t>#176</t>
         </is>
@@ -5810,7 +5812,7 @@
       <c r="M134" t="inlineStr"/>
     </row>
     <row r="135">
-      <c r="A135" t="inlineStr">
+      <c r="A135" s="1" t="inlineStr">
         <is>
           <t>#177</t>
         </is>
@@ -5849,7 +5851,7 @@
       <c r="M135" t="inlineStr"/>
     </row>
     <row r="136">
-      <c r="A136" t="inlineStr">
+      <c r="A136" s="1" t="inlineStr">
         <is>
           <t>#178</t>
         </is>
@@ -5888,7 +5890,7 @@
       <c r="M136" t="inlineStr"/>
     </row>
     <row r="137">
-      <c r="A137" t="inlineStr">
+      <c r="A137" s="1" t="inlineStr">
         <is>
           <t>#179</t>
         </is>
@@ -5927,7 +5929,7 @@
       <c r="M137" t="inlineStr"/>
     </row>
     <row r="138">
-      <c r="A138" t="inlineStr">
+      <c r="A138" s="1" t="inlineStr">
         <is>
           <t>#180</t>
         </is>
@@ -5968,7 +5970,7 @@
       </c>
     </row>
     <row r="139">
-      <c r="A139" t="inlineStr">
+      <c r="A139" s="1" t="inlineStr">
         <is>
           <t>#181</t>
         </is>
@@ -6007,7 +6009,7 @@
       <c r="M139" t="inlineStr"/>
     </row>
     <row r="140">
-      <c r="A140" t="inlineStr">
+      <c r="A140" s="1" t="inlineStr">
         <is>
           <t>#182</t>
         </is>
@@ -6046,7 +6048,7 @@
       <c r="M140" t="inlineStr"/>
     </row>
     <row r="141">
-      <c r="A141" t="inlineStr">
+      <c r="A141" s="1" t="inlineStr">
         <is>
           <t>#183</t>
         </is>
@@ -6085,7 +6087,7 @@
       <c r="M141" t="inlineStr"/>
     </row>
     <row r="142">
-      <c r="A142" t="inlineStr">
+      <c r="A142" s="1" t="inlineStr">
         <is>
           <t>#184</t>
         </is>
@@ -6124,7 +6126,7 @@
       <c r="M142" t="inlineStr"/>
     </row>
     <row r="143">
-      <c r="A143" t="inlineStr">
+      <c r="A143" s="1" t="inlineStr">
         <is>
           <t>#186</t>
         </is>
@@ -6163,7 +6165,7 @@
       <c r="M143" t="inlineStr"/>
     </row>
     <row r="144">
-      <c r="A144" t="inlineStr">
+      <c r="A144" s="1" t="inlineStr">
         <is>
           <t>#187</t>
         </is>
@@ -6202,7 +6204,7 @@
       <c r="M144" t="inlineStr"/>
     </row>
     <row r="145">
-      <c r="A145" t="inlineStr">
+      <c r="A145" s="1" t="inlineStr">
         <is>
           <t>#188</t>
         </is>
@@ -6241,7 +6243,7 @@
       <c r="M145" t="inlineStr"/>
     </row>
     <row r="146">
-      <c r="A146" t="inlineStr">
+      <c r="A146" s="1" t="inlineStr">
         <is>
           <t>#189</t>
         </is>
@@ -6280,7 +6282,7 @@
       <c r="M146" t="inlineStr"/>
     </row>
     <row r="147">
-      <c r="A147" t="inlineStr">
+      <c r="A147" s="1" t="inlineStr">
         <is>
           <t>#190</t>
         </is>
@@ -6319,7 +6321,7 @@
       <c r="M147" t="inlineStr"/>
     </row>
     <row r="148">
-      <c r="A148" t="inlineStr">
+      <c r="A148" s="1" t="inlineStr">
         <is>
           <t>#191</t>
         </is>
@@ -6358,7 +6360,7 @@
       <c r="M148" t="inlineStr"/>
     </row>
     <row r="149">
-      <c r="A149" t="inlineStr">
+      <c r="A149" s="1" t="inlineStr">
         <is>
           <t>#192</t>
         </is>
@@ -6397,7 +6399,7 @@
       <c r="M149" t="inlineStr"/>
     </row>
     <row r="150">
-      <c r="A150" t="inlineStr">
+      <c r="A150" s="1" t="inlineStr">
         <is>
           <t>#193</t>
         </is>
@@ -6440,7 +6442,7 @@
       </c>
     </row>
     <row r="151">
-      <c r="A151" t="inlineStr">
+      <c r="A151" s="1" t="inlineStr">
         <is>
           <t>#194</t>
         </is>
@@ -6479,7 +6481,7 @@
       <c r="M151" t="inlineStr"/>
     </row>
     <row r="152">
-      <c r="A152" t="inlineStr">
+      <c r="A152" s="1" t="inlineStr">
         <is>
           <t>#195</t>
         </is>
@@ -6520,7 +6522,7 @@
       </c>
     </row>
     <row r="153">
-      <c r="A153" t="inlineStr">
+      <c r="A153" s="1" t="inlineStr">
         <is>
           <t>#196</t>
         </is>
@@ -6559,13 +6561,13 @@
       <c r="M153" t="inlineStr"/>
     </row>
     <row r="154">
-      <c r="A154" t="inlineStr">
+      <c r="A154" s="1" t="inlineStr">
         <is>
           <t>#197</t>
         </is>
       </c>
       <c r="B154" t="n">
-        <v>61</v>
+        <v>999</v>
       </c>
       <c r="C154" t="n">
         <v>0</v>
@@ -6598,7 +6600,7 @@
       <c r="M154" t="inlineStr"/>
     </row>
     <row r="155">
-      <c r="A155" t="inlineStr">
+      <c r="A155" s="1" t="inlineStr">
         <is>
           <t>#198</t>
         </is>
@@ -6637,7 +6639,7 @@
       <c r="M155" t="inlineStr"/>
     </row>
     <row r="156">
-      <c r="A156" t="inlineStr">
+      <c r="A156" s="1" t="inlineStr">
         <is>
           <t>#199</t>
         </is>
@@ -6676,7 +6678,7 @@
       <c r="M156" t="inlineStr"/>
     </row>
     <row r="157">
-      <c r="A157" t="inlineStr">
+      <c r="A157" s="1" t="inlineStr">
         <is>
           <t>#200</t>
         </is>
@@ -6715,7 +6717,7 @@
       <c r="M157" t="inlineStr"/>
     </row>
     <row r="158">
-      <c r="A158" t="inlineStr">
+      <c r="A158" s="1" t="inlineStr">
         <is>
           <t>#201</t>
         </is>
@@ -6754,7 +6756,7 @@
       <c r="M158" t="inlineStr"/>
     </row>
     <row r="159">
-      <c r="A159" t="inlineStr">
+      <c r="A159" s="1" t="inlineStr">
         <is>
           <t>#202</t>
         </is>
@@ -6793,7 +6795,7 @@
       <c r="M159" t="inlineStr"/>
     </row>
     <row r="160">
-      <c r="A160" t="inlineStr">
+      <c r="A160" s="1" t="inlineStr">
         <is>
           <t>#203</t>
         </is>
@@ -6832,7 +6834,7 @@
       <c r="M160" t="inlineStr"/>
     </row>
     <row r="161">
-      <c r="A161" t="inlineStr">
+      <c r="A161" s="1" t="inlineStr">
         <is>
           <t>#204</t>
         </is>
@@ -6871,7 +6873,7 @@
       <c r="M161" t="inlineStr"/>
     </row>
     <row r="162">
-      <c r="A162" t="inlineStr">
+      <c r="A162" s="1" t="inlineStr">
         <is>
           <t>#205</t>
         </is>
@@ -6910,7 +6912,7 @@
       <c r="M162" t="inlineStr"/>
     </row>
     <row r="163">
-      <c r="A163" t="inlineStr">
+      <c r="A163" s="1" t="inlineStr">
         <is>
           <t>#206</t>
         </is>
@@ -6949,7 +6951,7 @@
       <c r="M163" t="inlineStr"/>
     </row>
     <row r="164">
-      <c r="A164" t="inlineStr">
+      <c r="A164" s="1" t="inlineStr">
         <is>
           <t>#207</t>
         </is>
@@ -6988,7 +6990,7 @@
       <c r="M164" t="inlineStr"/>
     </row>
     <row r="165">
-      <c r="A165" t="inlineStr">
+      <c r="A165" s="1" t="inlineStr">
         <is>
           <t>#208</t>
         </is>
@@ -7027,7 +7029,7 @@
       <c r="M165" t="inlineStr"/>
     </row>
     <row r="166">
-      <c r="A166" t="inlineStr">
+      <c r="A166" s="1" t="inlineStr">
         <is>
           <t>#209</t>
         </is>
@@ -7066,7 +7068,7 @@
       <c r="M166" t="inlineStr"/>
     </row>
     <row r="167">
-      <c r="A167" t="inlineStr">
+      <c r="A167" s="1" t="inlineStr">
         <is>
           <t>#210</t>
         </is>
@@ -7107,7 +7109,7 @@
       <c r="M167" t="inlineStr"/>
     </row>
     <row r="168">
-      <c r="A168" t="inlineStr">
+      <c r="A168" s="1" t="inlineStr">
         <is>
           <t>#211</t>
         </is>
@@ -7146,7 +7148,7 @@
       <c r="M168" t="inlineStr"/>
     </row>
     <row r="169">
-      <c r="A169" t="inlineStr">
+      <c r="A169" s="1" t="inlineStr">
         <is>
           <t>#212</t>
         </is>
@@ -7185,7 +7187,7 @@
       <c r="M169" t="inlineStr"/>
     </row>
     <row r="170">
-      <c r="A170" t="inlineStr">
+      <c r="A170" s="1" t="inlineStr">
         <is>
           <t>#213</t>
         </is>
@@ -7216,7 +7218,7 @@
       <c r="M170" t="inlineStr"/>
     </row>
     <row r="171">
-      <c r="A171" t="inlineStr">
+      <c r="A171" s="1" t="inlineStr">
         <is>
           <t>#214</t>
         </is>
@@ -7255,7 +7257,7 @@
       <c r="M171" t="inlineStr"/>
     </row>
     <row r="172">
-      <c r="A172" t="inlineStr">
+      <c r="A172" s="1" t="inlineStr">
         <is>
           <t>#215</t>
         </is>
@@ -7294,7 +7296,7 @@
       <c r="M172" t="inlineStr"/>
     </row>
     <row r="173">
-      <c r="A173" t="inlineStr">
+      <c r="A173" s="1" t="inlineStr">
         <is>
           <t>#216</t>
         </is>
@@ -7333,7 +7335,7 @@
       <c r="M173" t="inlineStr"/>
     </row>
     <row r="174">
-      <c r="A174" t="inlineStr">
+      <c r="A174" s="1" t="inlineStr">
         <is>
           <t>#217</t>
         </is>
@@ -7372,7 +7374,7 @@
       <c r="M174" t="inlineStr"/>
     </row>
     <row r="175">
-      <c r="A175" t="inlineStr">
+      <c r="A175" s="1" t="inlineStr">
         <is>
           <t>#218</t>
         </is>
@@ -7409,7 +7411,7 @@
       <c r="M175" t="inlineStr"/>
     </row>
     <row r="176">
-      <c r="A176" t="inlineStr">
+      <c r="A176" s="1" t="inlineStr">
         <is>
           <t>#219</t>
         </is>
@@ -7448,7 +7450,7 @@
       <c r="M176" t="inlineStr"/>
     </row>
     <row r="177">
-      <c r="A177" t="inlineStr">
+      <c r="A177" s="1" t="inlineStr">
         <is>
           <t>#220</t>
         </is>
@@ -7487,7 +7489,7 @@
       <c r="M177" t="inlineStr"/>
     </row>
     <row r="178">
-      <c r="A178" t="inlineStr">
+      <c r="A178" s="1" t="inlineStr">
         <is>
           <t>#221</t>
         </is>
@@ -7524,7 +7526,7 @@
       <c r="M178" t="inlineStr"/>
     </row>
     <row r="179">
-      <c r="A179" t="inlineStr">
+      <c r="A179" s="1" t="inlineStr">
         <is>
           <t>#222</t>
         </is>
@@ -7563,7 +7565,7 @@
       <c r="M179" t="inlineStr"/>
     </row>
     <row r="180">
-      <c r="A180" t="inlineStr">
+      <c r="A180" s="1" t="inlineStr">
         <is>
           <t>#223</t>
         </is>
@@ -7602,7 +7604,7 @@
       <c r="M180" t="inlineStr"/>
     </row>
     <row r="181">
-      <c r="A181" t="inlineStr">
+      <c r="A181" s="1" t="inlineStr">
         <is>
           <t>#224</t>
         </is>
@@ -7641,7 +7643,7 @@
       <c r="M181" t="inlineStr"/>
     </row>
     <row r="182">
-      <c r="A182" t="inlineStr">
+      <c r="A182" s="1" t="inlineStr">
         <is>
           <t>#225</t>
         </is>
@@ -7680,7 +7682,7 @@
       <c r="M182" t="inlineStr"/>
     </row>
     <row r="183">
-      <c r="A183" t="inlineStr">
+      <c r="A183" s="1" t="inlineStr">
         <is>
           <t>#227</t>
         </is>
@@ -7719,7 +7721,7 @@
       <c r="M183" t="inlineStr"/>
     </row>
     <row r="184">
-      <c r="A184" t="inlineStr">
+      <c r="A184" s="1" t="inlineStr">
         <is>
           <t>#228</t>
         </is>
@@ -7758,7 +7760,7 @@
       <c r="M184" t="inlineStr"/>
     </row>
     <row r="185">
-      <c r="A185" t="inlineStr">
+      <c r="A185" s="1" t="inlineStr">
         <is>
           <t>#229</t>
         </is>
@@ -7797,7 +7799,7 @@
       <c r="M185" t="inlineStr"/>
     </row>
     <row r="186">
-      <c r="A186" t="inlineStr">
+      <c r="A186" s="1" t="inlineStr">
         <is>
           <t>#230</t>
         </is>
@@ -7836,7 +7838,7 @@
       <c r="M186" t="inlineStr"/>
     </row>
     <row r="187">
-      <c r="A187" t="inlineStr">
+      <c r="A187" s="1" t="inlineStr">
         <is>
           <t>#231</t>
         </is>
@@ -7875,7 +7877,7 @@
       <c r="M187" t="inlineStr"/>
     </row>
     <row r="188">
-      <c r="A188" t="inlineStr">
+      <c r="A188" s="1" t="inlineStr">
         <is>
           <t>#232</t>
         </is>
@@ -7914,7 +7916,7 @@
       <c r="M188" t="inlineStr"/>
     </row>
     <row r="189">
-      <c r="A189" t="inlineStr">
+      <c r="A189" s="1" t="inlineStr">
         <is>
           <t>#233</t>
         </is>
@@ -7955,7 +7957,7 @@
       </c>
     </row>
     <row r="190">
-      <c r="A190" t="inlineStr">
+      <c r="A190" s="1" t="inlineStr">
         <is>
           <t>#234</t>
         </is>
@@ -7994,7 +7996,7 @@
       <c r="M190" t="inlineStr"/>
     </row>
     <row r="191">
-      <c r="A191" t="inlineStr">
+      <c r="A191" s="1" t="inlineStr">
         <is>
           <t>#235</t>
         </is>
@@ -8033,7 +8035,7 @@
       <c r="M191" t="inlineStr"/>
     </row>
     <row r="192">
-      <c r="A192" t="inlineStr">
+      <c r="A192" s="1" t="inlineStr">
         <is>
           <t>#236</t>
         </is>
@@ -8072,7 +8074,7 @@
       <c r="M192" t="inlineStr"/>
     </row>
     <row r="193">
-      <c r="A193" t="inlineStr">
+      <c r="A193" s="1" t="inlineStr">
         <is>
           <t>#237</t>
         </is>
@@ -8111,7 +8113,7 @@
       <c r="M193" t="inlineStr"/>
     </row>
     <row r="194">
-      <c r="A194" t="inlineStr">
+      <c r="A194" s="1" t="inlineStr">
         <is>
           <t>#238</t>
         </is>
@@ -8150,7 +8152,7 @@
       <c r="M194" t="inlineStr"/>
     </row>
     <row r="195">
-      <c r="A195" t="inlineStr">
+      <c r="A195" s="1" t="inlineStr">
         <is>
           <t>#239</t>
         </is>
@@ -8189,7 +8191,7 @@
       <c r="M195" t="inlineStr"/>
     </row>
     <row r="196">
-      <c r="A196" t="inlineStr">
+      <c r="A196" s="1" t="inlineStr">
         <is>
           <t>#240</t>
         </is>
@@ -8228,7 +8230,7 @@
       <c r="M196" t="inlineStr"/>
     </row>
     <row r="197">
-      <c r="A197" t="inlineStr">
+      <c r="A197" s="1" t="inlineStr">
         <is>
           <t>#241</t>
         </is>
@@ -8267,7 +8269,7 @@
       <c r="M197" t="inlineStr"/>
     </row>
     <row r="198">
-      <c r="A198" t="inlineStr">
+      <c r="A198" s="1" t="inlineStr">
         <is>
           <t>#242</t>
         </is>
@@ -8306,7 +8308,7 @@
       <c r="M198" t="inlineStr"/>
     </row>
     <row r="199">
-      <c r="A199" t="inlineStr">
+      <c r="A199" s="1" t="inlineStr">
         <is>
           <t>#243</t>
         </is>
@@ -8345,7 +8347,7 @@
       <c r="M199" t="inlineStr"/>
     </row>
     <row r="200">
-      <c r="A200" t="inlineStr">
+      <c r="A200" s="1" t="inlineStr">
         <is>
           <t>#244</t>
         </is>
@@ -8382,7 +8384,7 @@
       <c r="M200" t="inlineStr"/>
     </row>
     <row r="201">
-      <c r="A201" t="inlineStr">
+      <c r="A201" s="1" t="inlineStr">
         <is>
           <t>#245</t>
         </is>
@@ -8421,7 +8423,7 @@
       <c r="M201" t="inlineStr"/>
     </row>
     <row r="202">
-      <c r="A202" t="inlineStr">
+      <c r="A202" s="1" t="inlineStr">
         <is>
           <t>#246</t>
         </is>
@@ -8460,7 +8462,7 @@
       <c r="M202" t="inlineStr"/>
     </row>
     <row r="203">
-      <c r="A203" t="inlineStr">
+      <c r="A203" s="1" t="inlineStr">
         <is>
           <t>#248</t>
         </is>
@@ -8499,7 +8501,7 @@
       </c>
     </row>
     <row r="204">
-      <c r="A204" t="inlineStr">
+      <c r="A204" s="1" t="inlineStr">
         <is>
           <t>#249</t>
         </is>
@@ -8538,7 +8540,7 @@
       <c r="M204" t="inlineStr"/>
     </row>
     <row r="205">
-      <c r="A205" t="inlineStr">
+      <c r="A205" s="1" t="inlineStr">
         <is>
           <t>#250</t>
         </is>
@@ -8577,7 +8579,7 @@
       <c r="M205" t="inlineStr"/>
     </row>
     <row r="206">
-      <c r="A206" t="inlineStr">
+      <c r="A206" s="1" t="inlineStr">
         <is>
           <t>#251</t>
         </is>
@@ -8616,7 +8618,7 @@
       <c r="M206" t="inlineStr"/>
     </row>
     <row r="207">
-      <c r="A207" t="inlineStr">
+      <c r="A207" s="1" t="inlineStr">
         <is>
           <t>#252</t>
         </is>
@@ -8655,7 +8657,7 @@
       <c r="M207" t="inlineStr"/>
     </row>
     <row r="208">
-      <c r="A208" t="inlineStr">
+      <c r="A208" s="1" t="inlineStr">
         <is>
           <t>#253</t>
         </is>
@@ -8694,7 +8696,7 @@
       <c r="M208" t="inlineStr"/>
     </row>
     <row r="209">
-      <c r="A209" t="inlineStr">
+      <c r="A209" s="1" t="inlineStr">
         <is>
           <t>#254</t>
         </is>
@@ -8733,7 +8735,7 @@
       <c r="M209" t="inlineStr"/>
     </row>
     <row r="210">
-      <c r="A210" t="inlineStr">
+      <c r="A210" s="1" t="inlineStr">
         <is>
           <t>#255</t>
         </is>
@@ -8772,7 +8774,7 @@
       <c r="M210" t="inlineStr"/>
     </row>
     <row r="211">
-      <c r="A211" t="inlineStr">
+      <c r="A211" s="1" t="inlineStr">
         <is>
           <t>#256</t>
         </is>
@@ -8811,7 +8813,7 @@
       <c r="M211" t="inlineStr"/>
     </row>
     <row r="212">
-      <c r="A212" t="inlineStr">
+      <c r="A212" s="1" t="inlineStr">
         <is>
           <t>#257</t>
         </is>
@@ -8850,7 +8852,7 @@
       <c r="M212" t="inlineStr"/>
     </row>
     <row r="213">
-      <c r="A213" t="inlineStr">
+      <c r="A213" s="1" t="inlineStr">
         <is>
           <t>#258</t>
         </is>
@@ -8889,7 +8891,7 @@
       <c r="M213" t="inlineStr"/>
     </row>
     <row r="214">
-      <c r="A214" t="inlineStr">
+      <c r="A214" s="1" t="inlineStr">
         <is>
           <t>#259</t>
         </is>
@@ -8926,7 +8928,7 @@
       <c r="M214" t="inlineStr"/>
     </row>
     <row r="215">
-      <c r="A215" t="inlineStr">
+      <c r="A215" s="1" t="inlineStr">
         <is>
           <t>#260</t>
         </is>
@@ -8965,7 +8967,7 @@
       <c r="M215" t="inlineStr"/>
     </row>
     <row r="216">
-      <c r="A216" t="inlineStr">
+      <c r="A216" s="1" t="inlineStr">
         <is>
           <t>#261</t>
         </is>
@@ -9004,7 +9006,7 @@
       <c r="M216" t="inlineStr"/>
     </row>
     <row r="217">
-      <c r="A217" t="inlineStr">
+      <c r="A217" s="1" t="inlineStr">
         <is>
           <t>#262</t>
         </is>
@@ -9043,7 +9045,7 @@
       <c r="M217" t="inlineStr"/>
     </row>
     <row r="218">
-      <c r="A218" t="inlineStr">
+      <c r="A218" s="1" t="inlineStr">
         <is>
           <t>#264</t>
         </is>
@@ -9084,7 +9086,7 @@
       </c>
     </row>
     <row r="219">
-      <c r="A219" t="inlineStr">
+      <c r="A219" s="1" t="inlineStr">
         <is>
           <t>#265</t>
         </is>
@@ -9125,7 +9127,7 @@
       </c>
     </row>
     <row r="220">
-      <c r="A220" t="inlineStr">
+      <c r="A220" s="1" t="inlineStr">
         <is>
           <t>#266</t>
         </is>
@@ -9164,7 +9166,7 @@
       <c r="M220" t="inlineStr"/>
     </row>
     <row r="221">
-      <c r="A221" t="inlineStr">
+      <c r="A221" s="1" t="inlineStr">
         <is>
           <t>#267</t>
         </is>
@@ -9203,7 +9205,7 @@
       <c r="M221" t="inlineStr"/>
     </row>
     <row r="222">
-      <c r="A222" t="inlineStr">
+      <c r="A222" s="1" t="inlineStr">
         <is>
           <t>#268</t>
         </is>
@@ -9242,7 +9244,7 @@
       <c r="M222" t="inlineStr"/>
     </row>
     <row r="223">
-      <c r="A223" t="inlineStr">
+      <c r="A223" s="1" t="inlineStr">
         <is>
           <t>#269</t>
         </is>
@@ -9281,7 +9283,7 @@
       <c r="M223" t="inlineStr"/>
     </row>
     <row r="224">
-      <c r="A224" t="inlineStr">
+      <c r="A224" s="1" t="inlineStr">
         <is>
           <t>#270</t>
         </is>
@@ -9320,7 +9322,7 @@
       <c r="M224" t="inlineStr"/>
     </row>
     <row r="225">
-      <c r="A225" t="inlineStr">
+      <c r="A225" s="1" t="inlineStr">
         <is>
           <t>#271</t>
         </is>
@@ -9359,7 +9361,7 @@
       <c r="M225" t="inlineStr"/>
     </row>
     <row r="226">
-      <c r="A226" t="inlineStr">
+      <c r="A226" s="1" t="inlineStr">
         <is>
           <t>#272</t>
         </is>
@@ -9398,7 +9400,7 @@
       <c r="M226" t="inlineStr"/>
     </row>
     <row r="227">
-      <c r="A227" t="inlineStr">
+      <c r="A227" s="1" t="inlineStr">
         <is>
           <t>#273</t>
         </is>
@@ -9437,7 +9439,7 @@
       <c r="M227" t="inlineStr"/>
     </row>
     <row r="228">
-      <c r="A228" t="inlineStr">
+      <c r="A228" s="1" t="inlineStr">
         <is>
           <t>#274</t>
         </is>
@@ -9474,7 +9476,7 @@
       <c r="M228" t="inlineStr"/>
     </row>
     <row r="229">
-      <c r="A229" t="inlineStr">
+      <c r="A229" s="1" t="inlineStr">
         <is>
           <t>#275</t>
         </is>
@@ -9513,7 +9515,7 @@
       <c r="M229" t="inlineStr"/>
     </row>
     <row r="230">
-      <c r="A230" t="inlineStr">
+      <c r="A230" s="1" t="inlineStr">
         <is>
           <t>#276</t>
         </is>
@@ -9552,7 +9554,7 @@
       </c>
     </row>
     <row r="231">
-      <c r="A231" t="inlineStr">
+      <c r="A231" s="1" t="inlineStr">
         <is>
           <t>#277</t>
         </is>
@@ -9591,7 +9593,7 @@
       <c r="M231" t="inlineStr"/>
     </row>
     <row r="232">
-      <c r="A232" t="inlineStr">
+      <c r="A232" s="1" t="inlineStr">
         <is>
           <t>#280</t>
         </is>
@@ -9630,7 +9632,7 @@
       <c r="M232" t="inlineStr"/>
     </row>
     <row r="233">
-      <c r="A233" t="inlineStr">
+      <c r="A233" s="1" t="inlineStr">
         <is>
           <t>#281</t>
         </is>
@@ -9669,7 +9671,7 @@
       <c r="M233" t="inlineStr"/>
     </row>
     <row r="234">
-      <c r="A234" t="inlineStr">
+      <c r="A234" s="1" t="inlineStr">
         <is>
           <t>#282</t>
         </is>
@@ -9708,7 +9710,7 @@
       <c r="M234" t="inlineStr"/>
     </row>
     <row r="235">
-      <c r="A235" t="inlineStr">
+      <c r="A235" s="1" t="inlineStr">
         <is>
           <t>#283</t>
         </is>
@@ -9747,7 +9749,7 @@
       <c r="M235" t="inlineStr"/>
     </row>
     <row r="236">
-      <c r="A236" t="inlineStr">
+      <c r="A236" s="1" t="inlineStr">
         <is>
           <t>#284</t>
         </is>
@@ -9786,7 +9788,7 @@
       <c r="M236" t="inlineStr"/>
     </row>
     <row r="237">
-      <c r="A237" t="inlineStr">
+      <c r="A237" s="1" t="inlineStr">
         <is>
           <t>#285</t>
         </is>
@@ -9825,7 +9827,7 @@
       <c r="M237" t="inlineStr"/>
     </row>
     <row r="238">
-      <c r="A238" t="inlineStr">
+      <c r="A238" s="1" t="inlineStr">
         <is>
           <t>#286</t>
         </is>
@@ -9864,7 +9866,7 @@
       <c r="M238" t="inlineStr"/>
     </row>
     <row r="239">
-      <c r="A239" t="inlineStr">
+      <c r="A239" s="1" t="inlineStr">
         <is>
           <t>#287</t>
         </is>
@@ -9903,7 +9905,7 @@
       <c r="M239" t="inlineStr"/>
     </row>
     <row r="240">
-      <c r="A240" t="inlineStr">
+      <c r="A240" s="1" t="inlineStr">
         <is>
           <t>#288</t>
         </is>
@@ -9942,7 +9944,7 @@
       <c r="M240" t="inlineStr"/>
     </row>
     <row r="241">
-      <c r="A241" t="inlineStr">
+      <c r="A241" s="1" t="inlineStr">
         <is>
           <t>#289</t>
         </is>
@@ -9981,7 +9983,7 @@
       <c r="M241" t="inlineStr"/>
     </row>
     <row r="242">
-      <c r="A242" t="inlineStr">
+      <c r="A242" s="1" t="inlineStr">
         <is>
           <t>#290</t>
         </is>
@@ -10020,7 +10022,7 @@
       <c r="M242" t="inlineStr"/>
     </row>
     <row r="243">
-      <c r="A243" t="inlineStr">
+      <c r="A243" s="1" t="inlineStr">
         <is>
           <t>#291</t>
         </is>
@@ -10059,7 +10061,7 @@
       <c r="M243" t="inlineStr"/>
     </row>
     <row r="244">
-      <c r="A244" t="inlineStr">
+      <c r="A244" s="1" t="inlineStr">
         <is>
           <t>#292</t>
         </is>
@@ -10098,7 +10100,7 @@
       <c r="M244" t="inlineStr"/>
     </row>
     <row r="245">
-      <c r="A245" t="inlineStr">
+      <c r="A245" s="1" t="inlineStr">
         <is>
           <t>#293</t>
         </is>
@@ -10137,15 +10139,13 @@
       <c r="M245" t="inlineStr"/>
     </row>
     <row r="246">
-      <c r="A246" t="inlineStr">
+      <c r="A246" s="1" t="inlineStr">
         <is>
           <t>#295</t>
         </is>
       </c>
-      <c r="B246" t="inlineStr">
-        <is>
-          <t>39</t>
-        </is>
+      <c r="B246" t="n">
+        <v>39</v>
       </c>
       <c r="C246" t="inlineStr"/>
       <c r="D246" t="inlineStr"/>
@@ -10159,6 +10159,117 @@
       <c r="L246" t="inlineStr"/>
       <c r="M246" t="inlineStr"/>
     </row>
+    <row r="247">
+      <c r="A247" s="1" t="inlineStr">
+        <is>
+          <t>#294</t>
+        </is>
+      </c>
+      <c r="B247" t="n">
+        <v>41</v>
+      </c>
+      <c r="C247" t="inlineStr"/>
+      <c r="D247" t="inlineStr"/>
+      <c r="E247" t="inlineStr"/>
+      <c r="F247" t="inlineStr"/>
+      <c r="G247" t="inlineStr"/>
+      <c r="H247" t="inlineStr"/>
+      <c r="I247" t="inlineStr"/>
+      <c r="J247" t="inlineStr"/>
+      <c r="K247" t="inlineStr"/>
+      <c r="L247" t="inlineStr"/>
+      <c r="M247" t="inlineStr"/>
+    </row>
+    <row r="248">
+      <c r="A248" s="1" t="inlineStr">
+        <is>
+          <t>#294</t>
+        </is>
+      </c>
+      <c r="B248" t="n">
+        <v>42</v>
+      </c>
+      <c r="C248" t="n">
+        <v>1</v>
+      </c>
+      <c r="D248" t="n">
+        <v>1</v>
+      </c>
+      <c r="E248" t="inlineStr"/>
+      <c r="F248" t="inlineStr"/>
+      <c r="G248" t="inlineStr"/>
+      <c r="H248" t="inlineStr"/>
+      <c r="I248" t="inlineStr"/>
+      <c r="J248" t="inlineStr"/>
+      <c r="K248" t="inlineStr"/>
+      <c r="L248" t="inlineStr"/>
+      <c r="M248" t="inlineStr"/>
+    </row>
+    <row r="249">
+      <c r="A249" s="1" t="inlineStr">
+        <is>
+          <t>#294</t>
+        </is>
+      </c>
+      <c r="B249" t="n">
+        <v>41</v>
+      </c>
+      <c r="C249" t="inlineStr"/>
+      <c r="D249" t="inlineStr"/>
+      <c r="E249" t="inlineStr"/>
+      <c r="F249" t="inlineStr"/>
+      <c r="G249" t="inlineStr"/>
+      <c r="H249" t="inlineStr"/>
+      <c r="I249" t="inlineStr"/>
+      <c r="J249" t="inlineStr"/>
+      <c r="K249" t="inlineStr"/>
+      <c r="L249" t="inlineStr"/>
+      <c r="M249" t="inlineStr"/>
+    </row>
+    <row r="250">
+      <c r="A250" s="1" t="inlineStr">
+        <is>
+          <t>#296</t>
+        </is>
+      </c>
+      <c r="B250" t="n">
+        <v>41</v>
+      </c>
+      <c r="C250" t="inlineStr"/>
+      <c r="D250" t="inlineStr"/>
+      <c r="E250" t="inlineStr"/>
+      <c r="F250" t="inlineStr"/>
+      <c r="G250" t="inlineStr"/>
+      <c r="H250" t="inlineStr"/>
+      <c r="I250" t="inlineStr"/>
+      <c r="J250" t="inlineStr"/>
+      <c r="K250" t="inlineStr"/>
+      <c r="L250" t="inlineStr"/>
+      <c r="M250" t="inlineStr"/>
+    </row>
+    <row r="251">
+      <c r="A251" s="1" t="inlineStr">
+        <is>
+          <t>#297</t>
+        </is>
+      </c>
+      <c r="B251" t="n">
+        <v>25</v>
+      </c>
+      <c r="C251" t="n">
+        <v>0</v>
+      </c>
+      <c r="D251" t="inlineStr"/>
+      <c r="E251" t="inlineStr"/>
+      <c r="F251" t="inlineStr"/>
+      <c r="G251" t="inlineStr"/>
+      <c r="H251" t="inlineStr"/>
+      <c r="I251" t="inlineStr"/>
+      <c r="J251" t="inlineStr"/>
+      <c r="K251" t="inlineStr"/>
+      <c r="L251" t="inlineStr"/>
+      <c r="M251" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>